<commit_message>
update version 1.1 again
</commit_message>
<xml_diff>
--- a/(주)형경산업_MES_WBS_Sheet.xlsx
+++ b/(주)형경산업_MES_WBS_Sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EasyFwGuy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_code\HK_SmartFactory_Wbs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10250" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="10250"/>
   </bookViews>
   <sheets>
     <sheet name="시스템 구성도" sheetId="5" r:id="rId1"/>
@@ -1797,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
@@ -1811,13 +1811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
   <dimension ref="A2:I1013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5679,7 +5676,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>